<commit_message>
Added list of materials
</commit_message>
<xml_diff>
--- a/Electrical Team Materials.xlsx
+++ b/Electrical Team Materials.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JMurp\OneDrive\Jeremy's Files\UC Berkeley\Junior Year\ChemE_Car_Electrical_Team_2019-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a3d7edea914486d7/Jeremy's Files/UC Berkeley/Junior Year/ChemE_Car_Electrical_Team_2019-2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7E11D6-F333-438C-AC7C-D6DD09AB02BA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{A058E713-CEB3-4E16-8B69-523D0DC93C66}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{5C3AE03C-AC65-4513-955E-826DAC5A9626}"/>
   </bookViews>

</xml_diff>